<commit_message>
Refactor: Split Problem Sheets into Homework, Labs, and Quizzes
</commit_message>
<xml_diff>
--- a/Plan for Weeks 1-11.xlsx
+++ b/Plan for Weeks 1-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cr777\Desktop\Teaching 2024-2025\MA22019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai21/Projects/Teaching/MA22019/ma22019_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED6FCE-0DD8-4CF7-9D52-FCE8E754E0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB150CFE-E60A-924A-8B54-1122AB58F95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E075B94F-C021-456F-8276-BABA43872CDF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{E075B94F-C021-456F-8276-BABA43872CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>Week 1</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Lecture 2</t>
   </si>
   <si>
-    <t>LOIL</t>
-  </si>
-  <si>
     <t>Week 2</t>
   </si>
   <si>
@@ -161,15 +158,6 @@
     <t>Visualising point pattern data</t>
   </si>
   <si>
-    <t>Analysis of Airbnb Data</t>
-  </si>
-  <si>
-    <t>Coursework 2023 - Question 1</t>
-  </si>
-  <si>
-    <t>Coursework 2023 - Question 2</t>
-  </si>
-  <si>
     <t>Revision Lecture</t>
   </si>
   <si>
@@ -183,13 +171,205 @@
   </si>
   <si>
     <t>PS8</t>
+  </si>
+  <si>
+    <t>Problems class</t>
+  </si>
+  <si>
+    <t>Analysis of Airbnb Data (LOIL)</t>
+  </si>
+  <si>
+    <t>Coursework 2023 - Question 1 (LOIL)</t>
+  </si>
+  <si>
+    <t>Coursework 2023 - Question 2(LOIL)</t>
+  </si>
+  <si>
+    <t>sentiment analysis with Jane Eyre data</t>
+  </si>
+  <si>
+    <t>Overview.Rmd</t>
+  </si>
+  <si>
+    <t>Example.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis NRFA Data for Bathford.Rmd</t>
+  </si>
+  <si>
+    <t>Data Cleaning and Wrangling.Rmd</t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>Combining Data Frames.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis Australian Weather.Rmd</t>
+  </si>
+  <si>
+    <t>Data Visualization (Part 1).Rmd</t>
+  </si>
+  <si>
+    <t>R demos</t>
+  </si>
+  <si>
+    <t>Analysis Tuscany Data.Rmd, Analysis NRFA Data for Bathford.Rmd</t>
+  </si>
+  <si>
+    <t>Live coding</t>
+  </si>
+  <si>
+    <t>Analysis of Airbnb Data.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Airbnb Data (Complete).Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Pet Data.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Pet Data (Complete).Rmd</t>
+  </si>
+  <si>
+    <t>Data Visualization (Part 2).Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of wind speed and direction for Bela Vista.Rmd, Change in Scale - Examples.Rmd</t>
+  </si>
+  <si>
+    <t>Change in Data Structure - Example.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Fire Data.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Fire Data (Complete).Rmd</t>
+  </si>
+  <si>
+    <t>Notes Week 4.Rmd</t>
+  </si>
+  <si>
+    <t>Text Data Analysis (Part 1).Rmd</t>
+  </si>
+  <si>
+    <t>no demo (Q&amp;A session)</t>
+  </si>
+  <si>
+    <t>Analysis of Jane Eyre.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Jane Eyre.Rmd, Comparison of Jane Eyre and Wuthering Heights.Rmd</t>
+  </si>
+  <si>
+    <t>NO lecture</t>
+  </si>
+  <si>
+    <t>No live coding</t>
+  </si>
+  <si>
+    <t>Text Data Analysis (Part 2).Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of the work by Charles Dickens.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Jane Austen.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Jane Austen (Complete).Rmd</t>
+  </si>
+  <si>
+    <t>Mentimeters</t>
+  </si>
+  <si>
+    <t>Analysis of German Temperature Data.Rmd</t>
+  </si>
+  <si>
+    <t>Spatial Data Analysis (Part 1).Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Sea Surface Temperature.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Sea Surface Temperature (Complete).Rmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 8 </t>
+  </si>
+  <si>
+    <t>Spatial Data Analysis (Part 2).Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Colorado Precipitation Data.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of Sea Surface Temperature Anomalies.Rmd</t>
+  </si>
+  <si>
+    <t>Spatial Data Analyis (Part 3).Rmd</t>
+  </si>
+  <si>
+    <t>WildFires.Rmd, Tornadoes.Rmd, London.Rmd</t>
+  </si>
+  <si>
+    <t>Revision Class.Rmd</t>
+  </si>
+  <si>
+    <t>Analysis of NYT articles.Rmd, Semi-variogram example.Rmd</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Computer Lab</t>
+  </si>
+  <si>
+    <t>Homework exercises</t>
+  </si>
+  <si>
+    <t>Tutorial Week 1.Rmd</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>No quiz</t>
+  </si>
+  <si>
+    <t>No homework</t>
+  </si>
+  <si>
+    <t>Quiz 1.Rmd</t>
+  </si>
+  <si>
+    <t>Homework 1.Rmd</t>
+  </si>
+  <si>
+    <t>Lab 1 .Rmd</t>
+  </si>
+  <si>
+    <t>Quiz 2.Rmd</t>
+  </si>
+  <si>
+    <t>Lab 2 .Rmd</t>
+  </si>
+  <si>
+    <t>Homework 2.Rmd</t>
+  </si>
+  <si>
+    <t>Quiz 3.Rmd</t>
+  </si>
+  <si>
+    <t>No Lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +379,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,8 +412,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,203 +740,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2289CA-5398-4079-921A-493A52018EDA}">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="43.1796875" customWidth="1"/>
-    <col min="4" max="4" width="62" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="J18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" t="s">
+        <v>97</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B17:D17"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major cleanup: reorganize solutions, fix warnings, remove BOMs
- Move 23 solution files to _solutions/ folder (Labs, Quizzes, Homework by week)
- Create data symlinks in _solutions pointing to Practice/Week X/data
- Rename Moodle Quiz folders to _Moodle Quiz (excluded from build)
- Rename Coursework folders to _Coursework (excluded from build)
- Remove BOMs from CSV files (DataCleaningExample1.csv, Income Texas.csv)
- Fix Practice/_metadata.yml theme path (relative instead of absolute)
- Remove citation('dplyr') from Bela Vista file (encoding issue)
- Add trailing newlines to all .qmd files
- Update coursework.qmd to static page (no auto-listing)
- Fix broken link in computing-assignments.qmd (point to GitHub PAT docs)
- Remove .quartoignore (not needed with _ prefix convention)
</commit_message>
<xml_diff>
--- a/Plan for Weeks 1-11.xlsx
+++ b/Plan for Weeks 1-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai21/Projects/Teaching/MA22019/ma22019_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4599DC-E750-FB44-8C39-CBEA3CE94066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35C533D-881C-2D4A-B4C4-A2546648D874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{E075B94F-C021-456F-8276-BABA43872CDF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>Week 1</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>No Lab</t>
+  </si>
+  <si>
+    <t>Office hour</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -439,9 +442,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -452,15 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,15 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,12 +481,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,7 +822,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -844,58 +844,58 @@
   <sheetData>
     <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="17" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="19"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="29"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -906,31 +906,31 @@
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="23" t="s">
+      <c r="J4" s="11"/>
+      <c r="K4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="18" t="s">
         <v>62</v>
       </c>
     </row>
@@ -941,31 +941,31 @@
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="15"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -976,31 +976,31 @@
       <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="15"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1011,33 +1011,33 @@
       <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="14" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1048,29 +1048,28 @@
       <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="15"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1079,29 +1078,28 @@
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="15"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1110,29 +1108,28 @@
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1141,29 +1138,28 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1172,64 +1168,66 @@
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="15"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>